<commit_message>
Add a cylinder ZylSchild, update pinout, change cycle sequence
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Layout_Map_Push_Type.xlsx
+++ b/DOCUMENTS/Layout_Map_Push_Type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PushType Controllino Mega" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
   <si>
     <t xml:space="preserve">PINOUT  TEST RIG</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZylSchild</t>
   </si>
   <si>
     <t xml:space="preserve">D9</t>
@@ -1092,7 +1095,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1104,7 +1107,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Output" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1180,9 +1183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>124560</xdr:colOff>
+      <xdr:colOff>124200</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>2990880</xdr:rowOff>
+      <xdr:rowOff>2990520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1196,7 +1199,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1044720" y="8396640"/>
-          <a:ext cx="4489920" cy="2842560"/>
+          <a:ext cx="4489560" cy="2842200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1218,8 +1221,8 @@
   </sheetPr>
   <dimension ref="B5:N50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1418,8 +1421,8 @@
       <c r="G18" s="16"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="17" t="s">
-        <v>16</v>
+      <c r="B19" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="13" t="n">
@@ -1429,7 +1432,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19" s="16"/>
     </row>
@@ -1445,13 +1448,13 @@
         <v>8</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20" s="16"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13" t="n">
@@ -1461,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G21" s="16"/>
       <c r="M21" s="19"/>
@@ -1469,7 +1472,7 @@
     </row>
     <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13" t="n">
@@ -1479,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G22" s="16"/>
       <c r="M22" s="20"/>
@@ -1487,7 +1490,7 @@
     </row>
     <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="13" t="n">
@@ -1495,7 +1498,7 @@
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G23" s="16"/>
       <c r="M23" s="20"/>
@@ -1503,7 +1506,7 @@
     </row>
     <row r="24" s="1" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -1515,51 +1518,51 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -1571,91 +1574,91 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="13" t="n">
         <v>25</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="13" t="n">
         <v>26</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="13" t="n">
         <v>27</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
     </row>
     <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="13" t="n">
         <v>28</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G32" s="15"/>
       <c r="M32" s="20"/>
@@ -1663,7 +1666,7 @@
     </row>
     <row r="33" s="1" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -1675,19 +1678,19 @@
     </row>
     <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G34" s="16"/>
       <c r="M34" s="20"/>
@@ -1695,20 +1698,20 @@
     </row>
     <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
@@ -1716,19 +1719,19 @@
     <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="33"/>
       <c r="C36" s="41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M36" s="20"/>
       <c r="N36" s="20"/>
@@ -1736,17 +1739,17 @@
     <row r="37" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="33"/>
       <c r="C37" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G37" s="44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="253.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1774,10 +1777,10 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
       <c r="J41" s="51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K41" s="51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
@@ -1789,10 +1792,10 @@
       <c r="E42" s="52"/>
       <c r="F42" s="53"/>
       <c r="J42" s="51" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K42" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
@@ -1804,10 +1807,10 @@
       <c r="E43" s="54"/>
       <c r="F43" s="55"/>
       <c r="J43" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K43" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M43" s="20"/>
       <c r="N43" s="20"/>
@@ -1819,10 +1822,10 @@
       <c r="E44" s="54"/>
       <c r="F44" s="55"/>
       <c r="J44" s="51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K44" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
@@ -1834,10 +1837,10 @@
       <c r="E45" s="54"/>
       <c r="F45" s="55"/>
       <c r="J45" s="51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K45" s="51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1847,10 +1850,10 @@
       <c r="E46" s="54"/>
       <c r="F46" s="55"/>
       <c r="J46" s="51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K46" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,10 +1863,10 @@
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
       <c r="J47" s="51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K47" s="51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,10 +1876,10 @@
       <c r="E48" s="54"/>
       <c r="F48" s="54"/>
       <c r="J48" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K48" s="51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M48" s="20"/>
       <c r="N48" s="20"/>
@@ -1888,10 +1891,10 @@
       <c r="E49" s="50"/>
       <c r="F49" s="50"/>
       <c r="J49" s="51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K49" s="51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M49" s="20"/>
       <c r="N49" s="20"/>
@@ -1903,10 +1906,10 @@
       <c r="E50" s="52"/>
       <c r="F50" s="53"/>
       <c r="J50" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K50" s="51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M50" s="20"/>
       <c r="N50" s="20"/>
@@ -1941,7 +1944,7 @@
   </sheetPr>
   <dimension ref="C4:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1950,7 +1953,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="58" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
   </cols>
@@ -1960,25 +1963,25 @@
     </row>
     <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="59" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="59" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D7" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="59" t="s">
         <v>92</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>91</v>
       </c>
       <c r="F7" s="59"/>
     </row>
@@ -1987,13 +1990,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2001,13 +2004,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="62" t="s">
         <v>96</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2035,10 +2038,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F12" s="62"/>
     </row>
@@ -2047,10 +2050,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="61" t="s">
         <v>99</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>98</v>
       </c>
       <c r="F13" s="62"/>
     </row>
@@ -2059,13 +2062,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F14" s="62" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2073,13 +2076,13 @@
         <v>17</v>
       </c>
       <c r="D15" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="62" t="s">
         <v>103</v>
-      </c>
-      <c r="E15" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="62" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2087,10 +2090,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="60" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F16" s="62"/>
     </row>
@@ -2099,10 +2102,10 @@
         <v>19</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F17" s="62"/>
     </row>
@@ -2112,7 +2115,7 @@
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="61" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F18" s="62"/>
     </row>
@@ -2122,7 +2125,7 @@
       </c>
       <c r="D19" s="60"/>
       <c r="E19" s="61" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F19" s="62"/>
     </row>
@@ -2140,10 +2143,10 @@
     </row>
     <row r="22" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C22" s="66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>

</xml_diff>

<commit_message>
Make auto mode endless, add blower valve, fix strap feed bug
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Layout_Map_Push_Type.xlsx
+++ b/DOCUMENTS/Layout_Map_Push_Type.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
   <si>
     <t xml:space="preserve">PINOUT  TEST RIG</t>
   </si>
@@ -99,10 +99,13 @@
     <t xml:space="preserve">D3</t>
   </si>
   <si>
+    <t xml:space="preserve">ZylAirBlower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
     <t xml:space="preserve">(unconnected valve)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D4</t>
   </si>
   <si>
     <t xml:space="preserve">D5</t>
@@ -899,11 +902,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1183,9 +1186,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>124200</xdr:colOff>
+      <xdr:colOff>123840</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>2990520</xdr:rowOff>
+      <xdr:rowOff>2990160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1199,7 +1202,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1044720" y="8396640"/>
-          <a:ext cx="4489560" cy="2842200"/>
+          <a:ext cx="4489200" cy="2841840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1222,7 +1225,7 @@
   <dimension ref="B5:N50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1341,10 +1344,10 @@
       <c r="G13" s="16"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="13" t="n">
         <v>5</v>
       </c>
@@ -1357,10 +1360,10 @@
       <c r="G14" s="16"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="18"/>
+      <c r="B15" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="17"/>
       <c r="D15" s="13" t="n">
         <v>6</v>
       </c>
@@ -1368,13 +1371,13 @@
         <v>8</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="16"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13" t="n">
@@ -1384,13 +1387,13 @@
         <v>8</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="16"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13" t="n">
@@ -1400,13 +1403,13 @@
         <v>8</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" s="16"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13" t="n">
@@ -1416,15 +1419,15 @@
         <v>8</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G18" s="16"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="C19" s="17"/>
       <c r="D19" s="13" t="n">
         <v>12</v>
       </c>
@@ -1432,15 +1435,15 @@
         <v>8</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G19" s="16"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="17"/>
       <c r="D20" s="13" t="n">
         <v>13</v>
       </c>
@@ -1448,13 +1451,13 @@
         <v>8</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G20" s="16"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13" t="n">
@@ -1464,7 +1467,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G21" s="16"/>
       <c r="M21" s="19"/>
@@ -1472,7 +1475,7 @@
     </row>
     <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13" t="n">
@@ -1482,23 +1485,23 @@
         <v>8</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G22" s="16"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="18"/>
+      <c r="B23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="17"/>
       <c r="D23" s="13" t="n">
         <v>16</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G23" s="16"/>
       <c r="M23" s="20"/>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="24" s="1" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -1518,51 +1521,51 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -1574,91 +1577,91 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="13" t="n">
         <v>25</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="13" t="n">
         <v>26</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="13" t="n">
         <v>27</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
     </row>
     <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="13" t="n">
         <v>28</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G32" s="15"/>
       <c r="M32" s="20"/>
@@ -1666,7 +1669,7 @@
     </row>
     <row r="33" s="1" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -1678,19 +1681,19 @@
     </row>
     <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G34" s="16"/>
       <c r="M34" s="20"/>
@@ -1698,20 +1701,20 @@
     </row>
     <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="39" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
@@ -1719,19 +1722,19 @@
     <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="33"/>
       <c r="C36" s="41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M36" s="20"/>
       <c r="N36" s="20"/>
@@ -1739,17 +1742,17 @@
     <row r="37" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="33"/>
       <c r="C37" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G37" s="44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="253.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1777,10 +1780,10 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
       <c r="J41" s="51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K41" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
@@ -1792,10 +1795,10 @@
       <c r="E42" s="52"/>
       <c r="F42" s="53"/>
       <c r="J42" s="51" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K42" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
@@ -1807,10 +1810,10 @@
       <c r="E43" s="54"/>
       <c r="F43" s="55"/>
       <c r="J43" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K43" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M43" s="20"/>
       <c r="N43" s="20"/>
@@ -1822,10 +1825,10 @@
       <c r="E44" s="54"/>
       <c r="F44" s="55"/>
       <c r="J44" s="51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K44" s="51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
@@ -1837,10 +1840,10 @@
       <c r="E45" s="54"/>
       <c r="F45" s="55"/>
       <c r="J45" s="51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K45" s="51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1850,10 +1853,10 @@
       <c r="E46" s="54"/>
       <c r="F46" s="55"/>
       <c r="J46" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K46" s="51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,10 +1866,10 @@
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
       <c r="J47" s="51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K47" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,10 +1879,10 @@
       <c r="E48" s="54"/>
       <c r="F48" s="54"/>
       <c r="J48" s="51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K48" s="51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M48" s="20"/>
       <c r="N48" s="20"/>
@@ -1891,10 +1894,10 @@
       <c r="E49" s="50"/>
       <c r="F49" s="50"/>
       <c r="J49" s="51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K49" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M49" s="20"/>
       <c r="N49" s="20"/>
@@ -1906,10 +1909,10 @@
       <c r="E50" s="52"/>
       <c r="F50" s="53"/>
       <c r="J50" s="51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K50" s="51" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M50" s="20"/>
       <c r="N50" s="20"/>
@@ -1963,25 +1966,25 @@
     </row>
     <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="59" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="59"/>
     </row>
@@ -1990,13 +1993,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2004,13 +2007,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="62" t="s">
         <v>97</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2038,10 +2041,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F12" s="62"/>
     </row>
@@ -2050,10 +2053,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="61" t="s">
         <v>100</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>99</v>
       </c>
       <c r="F13" s="62"/>
     </row>
@@ -2062,13 +2065,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F14" s="62" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2076,13 +2079,13 @@
         <v>17</v>
       </c>
       <c r="D15" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="62" t="s">
         <v>104</v>
-      </c>
-      <c r="E15" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="62" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2090,10 +2093,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="60" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F16" s="62"/>
     </row>
@@ -2102,10 +2105,10 @@
         <v>19</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F17" s="62"/>
     </row>
@@ -2115,7 +2118,7 @@
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="61" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F18" s="62"/>
     </row>
@@ -2125,7 +2128,7 @@
       </c>
       <c r="D19" s="60"/>
       <c r="E19" s="61" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F19" s="62"/>
     </row>
@@ -2143,10 +2146,10 @@
     </row>
     <row r="22" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C22" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D22" s="66" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>

</xml_diff>

<commit_message>
Update pinout map with pt100 sensor
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Layout_Map_Push_Type.xlsx
+++ b/DOCUMENTS/Layout_Map_Push_Type.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
   <si>
     <t>PINOUT  TEST RIG</t>
   </si>
@@ -235,9 +235,6 @@
     <t>+=BN, GND=BL</t>
   </si>
   <si>
-    <t>STEP_MODE_BUTTON</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>used for tool motor start</t>
-  </si>
-  <si>
     <t>STOP_BUTON</t>
   </si>
   <si>
@@ -410,6 +404,12 @@
   </si>
   <si>
     <t>INTERRUPT PIN</t>
+  </si>
+  <si>
+    <t>TEMP_SENSOR_PIN</t>
+  </si>
+  <si>
+    <t>PT100</t>
   </si>
 </sst>
 </file>
@@ -936,36 +936,6 @@
   </cellStyleXfs>
   <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1116,6 +1086,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1573,8 +1573,8 @@
   </sheetPr>
   <dimension ref="B6:N50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,688 +1582,690 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:7" s="13" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:7" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" s="13" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+    </row>
+    <row r="7" spans="2:7" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="16" t="s">
+      <c r="E8" s="63"/>
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10">
         <v>1</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20">
+      <c r="C11" s="9"/>
+      <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10">
         <v>3</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="2:7" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10">
         <v>4</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="2:7" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="20">
+      <c r="C14" s="14"/>
+      <c r="D14" s="10">
         <v>5</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="2:7" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="20">
+      <c r="C15" s="14"/>
+      <c r="D15" s="10">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="2:7" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20">
+      <c r="C16" s="9"/>
+      <c r="D16" s="10">
         <v>7</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10">
         <v>8</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10">
         <v>11</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="20">
+      <c r="C19" s="14"/>
+      <c r="D19" s="10">
         <v>12</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="23"/>
-    </row>
-    <row r="20" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="20">
+      <c r="C20" s="14"/>
+      <c r="D20" s="10">
         <v>13</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="23"/>
-    </row>
-    <row r="21" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10">
         <v>14</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-    </row>
-    <row r="22" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="G21" s="13"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+    </row>
+    <row r="22" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20">
+      <c r="C22" s="9"/>
+      <c r="D22" s="10">
         <v>15</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-    </row>
-    <row r="23" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
+      <c r="G22" s="13"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="20">
+      <c r="C23" s="14"/>
+      <c r="D23" s="10">
         <v>16</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-    </row>
-    <row r="24" spans="2:14" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="G23" s="13"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+    </row>
+    <row r="24" spans="2:14" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
     </row>
     <row r="27" spans="2:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="22"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10">
         <v>25</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10">
+        <v>26</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20">
-        <v>26</v>
-      </c>
-      <c r="E30" s="20" t="s">
+      <c r="G30" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10">
+        <v>27</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20">
-        <v>27</v>
-      </c>
-      <c r="E31" s="20" t="s">
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+    </row>
+    <row r="32" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10">
+        <v>28</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="22" t="s">
+      <c r="F32" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-    </row>
-    <row r="32" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
+      <c r="G32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+    </row>
+    <row r="33" spans="2:14" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20">
-        <v>28</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="21" t="s">
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+    </row>
+    <row r="34" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="22"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-    </row>
-    <row r="33" spans="2:14" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+      <c r="C34" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-    </row>
-    <row r="34" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="37" t="s">
+      <c r="D34" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="G34" s="13"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+    </row>
+    <row r="35" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="C35" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E35" s="32"/>
+      <c r="F35" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+    </row>
+    <row r="36" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="60"/>
+      <c r="C36" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="23"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-    </row>
-    <row r="35" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="41" t="s">
+      <c r="F36" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+    </row>
+    <row r="37" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="60"/>
+      <c r="C37" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D37" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43" t="s">
+      <c r="E37" s="32"/>
+      <c r="F37" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" s="1" customFormat="1" ht="253.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="39"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="42"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+    </row>
+    <row r="39" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="43"/>
+    </row>
+    <row r="40" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="43"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+    </row>
+    <row r="41" spans="2:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="J41" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-    </row>
-    <row r="36" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="C36" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-    </row>
-    <row r="37" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-      <c r="C37" s="41" t="s">
+      <c r="K41" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
+      <c r="J42" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="K42" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+    </row>
+    <row r="43" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="48"/>
+      <c r="J43" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="K43" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+    </row>
+    <row r="44" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="48"/>
+      <c r="J44" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" s="11" customFormat="1" ht="253.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="49"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="52"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-    </row>
-    <row r="39" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G39" s="53"/>
-    </row>
-    <row r="40" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G40" s="53"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-    </row>
-    <row r="41" spans="2:14" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="J41" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="K41" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-    </row>
-    <row r="42" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="56"/>
-      <c r="J42" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="K42" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-    </row>
-    <row r="43" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="58"/>
-      <c r="J43" s="54" t="s">
+      <c r="K44" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="K43" s="54" t="s">
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+    </row>
+    <row r="45" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="48"/>
+      <c r="J45" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-    </row>
-    <row r="44" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
-      <c r="J44" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="K44" s="54" t="s">
+      <c r="K45" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-    </row>
-    <row r="45" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
-      <c r="J45" s="54" t="s">
+    </row>
+    <row r="46" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="48"/>
+      <c r="J46" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="K45" s="54" t="s">
+      <c r="K46" s="44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:14" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="J46" s="54" t="s">
+    <row r="47" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="J47" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="K47" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="K46" s="54" t="s">
+    </row>
+    <row r="48" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="J48" s="44" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="60"/>
-      <c r="J47" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="K47" s="54" t="s">
+      <c r="K48" s="44" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="J48" s="54" t="s">
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+    </row>
+    <row r="49" spans="2:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="J49" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="K48" s="54" t="s">
+      <c r="K49" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-    </row>
-    <row r="49" spans="2:14" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="J49" s="54" t="s">
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+    </row>
+    <row r="50" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="46"/>
+      <c r="J50" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="K49" s="54" t="s">
+      <c r="K50" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-    </row>
-    <row r="50" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="56"/>
-      <c r="J50" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="K50" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="M50" s="27"/>
-      <c r="N50" s="27"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2279,11 +2281,11 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.31527777777777799"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="90" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;10&amp;F / &amp;D</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2299,7 +2301,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" style="61" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" style="51" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="1025" width="9.140625" customWidth="1"/>
@@ -2309,194 +2311,194 @@
       <c r="C4"/>
     </row>
     <row r="6" spans="3:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="67"/>
+      <c r="E6" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="62" t="s">
+    </row>
+    <row r="7" spans="3:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="D7" s="52" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="62" t="s">
+      <c r="E7" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="67"/>
+    </row>
+    <row r="8" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="53">
+        <v>0</v>
+      </c>
+      <c r="D8" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="E8" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="63">
-        <v>0</v>
-      </c>
-      <c r="D8" s="63" t="s">
+      <c r="F8" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="64" t="s">
+    </row>
+    <row r="9" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="53">
+        <v>1</v>
+      </c>
+      <c r="D9" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="E9" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="56">
+        <v>2</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="55"/>
+    </row>
+    <row r="11" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="56">
+        <v>3</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="55"/>
+    </row>
+    <row r="12" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="53">
+        <v>14</v>
+      </c>
+      <c r="D12" s="53" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="63">
-        <v>1</v>
-      </c>
-      <c r="D9" s="63" t="s">
+      <c r="E12" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="66">
-        <v>2</v>
-      </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="65"/>
-    </row>
-    <row r="11" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="66">
-        <v>3</v>
-      </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="65"/>
-    </row>
-    <row r="12" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="63">
-        <v>14</v>
-      </c>
-      <c r="D12" s="63" t="s">
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="53">
+        <v>15</v>
+      </c>
+      <c r="D13" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E13" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="53">
+        <v>16</v>
+      </c>
+      <c r="D14" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="65"/>
-    </row>
-    <row r="13" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="63">
-        <v>15</v>
-      </c>
-      <c r="D13" s="63" t="s">
+      <c r="E14" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="64" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="65"/>
-    </row>
-    <row r="14" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="63">
-        <v>16</v>
-      </c>
-      <c r="D14" s="63" t="s">
+      <c r="F14" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="64" t="s">
+    </row>
+    <row r="15" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="53">
+        <v>17</v>
+      </c>
+      <c r="D15" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="65" t="s">
+      <c r="E15" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="56">
+        <v>18</v>
+      </c>
+      <c r="D16" s="53" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="63">
-        <v>17</v>
-      </c>
-      <c r="D15" s="63" t="s">
+      <c r="E16" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="65" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="66">
-        <v>18</v>
-      </c>
-      <c r="D16" s="63" t="s">
+      <c r="F16" s="55"/>
+    </row>
+    <row r="17" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="56">
+        <v>19</v>
+      </c>
+      <c r="D17" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E17" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="65"/>
-    </row>
-    <row r="17" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="66">
-        <v>19</v>
-      </c>
-      <c r="D17" s="63" t="s">
+      <c r="F17" s="55"/>
+    </row>
+    <row r="18" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="56">
+        <v>20</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="67" t="s">
+      <c r="F18" s="55"/>
+    </row>
+    <row r="19" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="56">
+        <v>21</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="55"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="3:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="65"/>
-    </row>
-    <row r="18" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="66">
-        <v>20</v>
-      </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="64" t="s">
+      <c r="D22" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="65"/>
-    </row>
-    <row r="19" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="66">
-        <v>21</v>
-      </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19" s="65"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="3:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Update pinout map with pt100 sensor module
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Layout_Map_Push_Type.xlsx
+++ b/DOCUMENTS/Layout_Map_Push_Type.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>PINOUT  TEST RIG</t>
   </si>
@@ -238,18 +238,9 @@
     <t>A2</t>
   </si>
   <si>
-    <t>deactivated</t>
-  </si>
-  <si>
-    <t>START_BUTTON</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
-    <t>STOP_BUTON</t>
-  </si>
-  <si>
     <t>A0</t>
   </si>
   <si>
@@ -409,7 +400,13 @@
     <t>TEMP_SENSOR_PIN</t>
   </si>
   <si>
-    <t>PT100</t>
+    <t>PT100 Module 0...200°C  0…10V</t>
+  </si>
+  <si>
+    <t>deactivated (ex start_button)</t>
+  </si>
+  <si>
+    <t>deactivated (ex stop_button)</t>
   </si>
 </sst>
 </file>
@@ -1573,8 +1570,8 @@
   </sheetPr>
   <dimension ref="B6:N50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1580,7 @@
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="1025" width="11.42578125"/>
   </cols>
@@ -1961,7 +1958,7 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="10">
@@ -1974,12 +1971,12 @@
         <v>54</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>56</v>
+      <c r="B31" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="10">
@@ -1989,17 +1986,17 @@
         <v>49</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
     </row>
     <row r="32" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>58</v>
+      <c r="B32" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="10">
@@ -2009,17 +2006,17 @@
         <v>49</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
     </row>
     <row r="33" spans="2:14" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="59" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
@@ -2031,10 +2028,10 @@
     </row>
     <row r="34" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>33</v>
@@ -2043,7 +2040,7 @@
         <v>8</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G34" s="13"/>
       <c r="M34" s="17"/>
@@ -2051,7 +2048,7 @@
     </row>
     <row r="35" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="60" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>37</v>
@@ -2061,10 +2058,10 @@
       </c>
       <c r="E35" s="32"/>
       <c r="F35" s="33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -2072,7 +2069,7 @@
     <row r="36" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="60"/>
       <c r="C36" s="35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>33</v>
@@ -2081,10 +2078,10 @@
         <v>8</v>
       </c>
       <c r="F36" s="36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -2099,10 +2096,10 @@
       </c>
       <c r="E37" s="32"/>
       <c r="F37" s="37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:14" s="1" customFormat="1" ht="253.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2130,10 +2127,10 @@
       <c r="E41" s="61"/>
       <c r="F41" s="61"/>
       <c r="J41" s="44" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K41" s="44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
@@ -2148,7 +2145,7 @@
         <v>47</v>
       </c>
       <c r="K42" s="44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
@@ -2160,10 +2157,10 @@
       <c r="E43" s="47"/>
       <c r="F43" s="48"/>
       <c r="J43" s="44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K43" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
@@ -2178,7 +2175,7 @@
         <v>37</v>
       </c>
       <c r="K44" s="44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
@@ -2190,10 +2187,10 @@
       <c r="E45" s="47"/>
       <c r="F45" s="48"/>
       <c r="J45" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K45" s="44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="2:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2203,10 +2200,10 @@
       <c r="E46" s="47"/>
       <c r="F46" s="48"/>
       <c r="J46" s="44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K46" s="44" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2216,10 +2213,10 @@
       <c r="E47" s="49"/>
       <c r="F47" s="50"/>
       <c r="J47" s="44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K47" s="44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2229,10 +2226,10 @@
       <c r="E48" s="47"/>
       <c r="F48" s="47"/>
       <c r="J48" s="44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K48" s="44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
@@ -2244,10 +2241,10 @@
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
       <c r="J49" s="44" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K49" s="44" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
@@ -2259,10 +2256,10 @@
       <c r="E50" s="45"/>
       <c r="F50" s="46"/>
       <c r="J50" s="44" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K50" s="44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -2312,25 +2309,25 @@
     </row>
     <row r="6" spans="3:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="67" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" s="67"/>
       <c r="E6" s="52" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F6" s="67" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F7" s="67"/>
     </row>
@@ -2339,13 +2336,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2353,13 +2350,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" s="55" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2387,10 +2384,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F12" s="55"/>
     </row>
@@ -2399,10 +2396,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E13" s="54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F13" s="55"/>
     </row>
@@ -2411,13 +2408,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,13 +2422,13 @@
         <v>17</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F15" s="55" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,10 +2436,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F16" s="55"/>
     </row>
@@ -2451,10 +2448,10 @@
         <v>19</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F17" s="55"/>
     </row>
@@ -2464,7 +2461,7 @@
       </c>
       <c r="D18" s="53"/>
       <c r="E18" s="54" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F18" s="55"/>
     </row>
@@ -2474,7 +2471,7 @@
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="54" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F19" s="55"/>
     </row>
@@ -2492,10 +2489,10 @@
     </row>
     <row r="22" spans="3:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="68" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D22" s="68" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>

</xml_diff>